<commit_message>
Add time series data. Add tests and calibration methods for Heatrecovery, Spaceheater, Controller
</commit_message>
<xml_diff>
--- a/twin4build/test/data/configuration_template_1space_1v_1h_0c_test_new_layout_simple_naming.xlsx
+++ b/twin4build/test/data/configuration_template_1space_1v_1h_0c_test_new_layout_simple_naming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syddanskuni-my.sharepoint.com/personal/jabj_mmmi_sdu_dk/Documents/PhD_Project_Jakob/Twin4build/python/BuildingEnergyModel/BuildingEnergyModel/twin4build/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="327" documentId="8_{AAA6B40C-6A0C-4905-8430-5C49F148860B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{488770D2-7DCF-4780-8896-20C9618FC037}"/>
+  <xr:revisionPtr revIDLastSave="329" documentId="8_{AAA6B40C-6A0C-4905-8430-5C49F148860B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18CCF34B-5E17-45E2-9F01-3B8E69F841C4}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-105" windowWidth="38640" windowHeight="21240" activeTab="10" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
+    <workbookView xWindow="-38055" yWindow="585" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
   </bookViews>
   <sheets>
     <sheet name="Systems" sheetId="3" r:id="rId1"/>
@@ -402,9 +402,6 @@
     <t>Ø20-601b-2_temperature;Ø20-601b-2_CO2</t>
   </si>
   <si>
-    <t>CO2Concentration</t>
-  </si>
-  <si>
     <t>isExternal</t>
   </si>
   <si>
@@ -454,6 +451,9 @@
   </si>
   <si>
     <t>Space</t>
+  </si>
+  <si>
+    <t>Co2</t>
   </si>
 </sst>
 </file>
@@ -1012,39 +1012,39 @@
         <v>101</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>87</v>
@@ -1064,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D904F809-0565-4493-A542-77B590BDC86C}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,10 +1088,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
         <v>82</v>
@@ -1099,10 +1099,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
         <v>84</v>
@@ -1110,10 +1110,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
         <v>85</v>
@@ -1121,10 +1121,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" t="s">
         <v>86</v>
@@ -1132,10 +1132,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" t="s">
         <v>119</v>
-      </c>
-      <c r="B6" t="s">
-        <v>120</v>
       </c>
       <c r="C6" t="s">
         <v>87</v>
@@ -1194,10 +1194,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
         <v>89</v>
@@ -1236,7 +1236,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,7 +1267,7 @@
         <v>84</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1398,7 +1398,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1472,7 +1472,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>102</v>
@@ -1617,7 +1617,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>86</v>
@@ -1638,7 +1638,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>86</v>
@@ -6662,8 +6662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F9D35B-B713-4EC3-BA55-A4EE8F2F331C}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6743,7 +6743,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D2" t="s">
         <v>74</v>
@@ -12699,7 +12699,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B48:B1048576 B2:B46" xr:uid="{CDBF1DD2-FE2B-4960-AE5E-D5DDA44A6748}">
       <formula1>heating_system_names</formula1>
     </dataValidation>
@@ -12784,7 +12784,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D2" t="s">
         <v>73</v>
@@ -40309,7 +40309,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D2" t="s">
         <v>82</v>
@@ -40323,7 +40323,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Add calibration examples and data
</commit_message>
<xml_diff>
--- a/twin4build/test/data/configuration_template_1space_1v_1h_0c_test_new_layout_simple_naming.xlsx
+++ b/twin4build/test/data/configuration_template_1space_1v_1h_0c_test_new_layout_simple_naming.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syddanskuni-my.sharepoint.com/personal/jabj_mmmi_sdu_dk/Documents/PhD_Project_Jakob/Twin4build/python/BuildingEnergyModel/BuildingEnergyModel/twin4build/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="329" documentId="8_{AAA6B40C-6A0C-4905-8430-5C49F148860B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18CCF34B-5E17-45E2-9F01-3B8E69F841C4}"/>
+  <xr:revisionPtr revIDLastSave="538" documentId="8_{AAA6B40C-6A0C-4905-8430-5C49F148860B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA16BDFB-8A35-43B0-B96C-3A615FD10DFD}"/>
   <bookViews>
-    <workbookView xWindow="-38055" yWindow="585" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
   </bookViews>
   <sheets>
-    <sheet name="Systems" sheetId="3" r:id="rId1"/>
+    <sheet name="System" sheetId="3" r:id="rId1"/>
     <sheet name="BuildingSpace" sheetId="1" r:id="rId2"/>
     <sheet name="Damper" sheetId="4" r:id="rId3"/>
     <sheet name="SpaceHeater" sheetId="2" r:id="rId4"/>
@@ -32,21 +32,22 @@
   <definedNames>
     <definedName name="controller_options">Controller_options!$A$1:$A$3</definedName>
     <definedName name="cooling_coil_names">OFFSET(#REF!, 0, 0, COUNTA(#REF!)-1, 1)</definedName>
-    <definedName name="cooling_system_names">OFFSET(Systems!$C$2, 0, 0, COUNTA(Systems!$C:$C), 1)</definedName>
+    <definedName name="cooling_system_names">IF(COUNTA(System!$C:$C)&gt;1,OFFSET(System!$C$2, 0, 0, COUNTA(System!$C:$C)-1, 1),"")</definedName>
     <definedName name="count_name_occurences">_xlfn.LAMBDA(_xlpm.cell_,COUNTIF(ventilation_system_names,_xlpm.cell_)+COUNTIF(heating_system_names,_xlpm.cell_)+COUNTIF(cooling_system_names,_xlpm.cell_)+COUNTIF(damper_names,_xlpm.cell_)+COUNTIF(space_heater_names,_xlpm.cell_)+COUNTIF(valve_names,_xlpm.cell_)+COUNTIF(space_names,_xlpm.cell_)+COUNTIF(heating_coil_names,_xlpm.cell_)+COUNTIF(cooling_coil_names,_xlpm.cell_))</definedName>
     <definedName name="damper_names">OFFSET(Damper!$A$2, 0, 0, COUNTA(Damper!$A:$A), 1)</definedName>
-    <definedName name="heating_coil_names">OFFSET(Coil!$A$2, 0, 0, COUNTA(Coil!$A:$A), 1)</definedName>
-    <definedName name="heating_system_names">OFFSET(Systems!$B$2, 0, 0, COUNTA(Systems!$B:$B), 1)</definedName>
+    <definedName name="heating_coil_names">IF(COUNTA(Coil!$A:$A)&gt;1,OFFSET(Coil!$A$2, 0, 0, COUNTA(Coil!$A:$A), 1),"")</definedName>
+    <definedName name="heating_system_names">OFFSET(System!$B$2, 0, 0, COUNTA(System!$B:$B)-1, 1)</definedName>
     <definedName name="property_class">named_ranges!$A$2:$A$1048576</definedName>
     <definedName name="property_instance">Property!$A$2:$A$1048576</definedName>
     <definedName name="sheet_dampers">Damper!$1:$1048576</definedName>
     <definedName name="sheet_space_heaters">SpaceHeater!$1:$1048576</definedName>
     <definedName name="sheet_spaces">BuildingSpace!$1:$1048576</definedName>
-    <definedName name="sheet_systems">Systems!$1:$1048576</definedName>
+    <definedName name="sheet_systems">System!$1:$1048576</definedName>
     <definedName name="space_heater_names">OFFSET(SpaceHeater!#REF!, 0, 0, COUNTA(SpaceHeater!$A:$A), 1)</definedName>
     <definedName name="space_names">BuildingSpace!$A$2:$A$1048576</definedName>
+    <definedName name="system_names">_xlfn.VSTACK(ventilation_system_names,heating_system_names,cooling_system_names)</definedName>
     <definedName name="valve_names">Valve!$A$2:$A$1048576</definedName>
-    <definedName name="ventilation_system_names">Systems!$A$2:$A$1048576</definedName>
+    <definedName name="ventilation_system_names">IF(COUNTA(System!$A:$A)&gt;1,OFFSET(System!$A$2, 0, 0, COUNTA(System!$A:$A)-1, 1),"")</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -91,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="137">
   <si>
     <t>Ventilation system name</t>
   </si>
@@ -339,28 +340,10 @@
     <t>OpeningPosition</t>
   </si>
   <si>
-    <t>Ø20-601b-2_temperature</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
-    <t>Ø20-601b-2_CO2</t>
-  </si>
-  <si>
-    <t>Ø20-601b-2_radiator_valve_position</t>
-  </si>
-  <si>
-    <t>Ø20-601b-2_damper_position</t>
-  </si>
-  <si>
-    <t>Ø20-601b-2_shading_position</t>
-  </si>
-  <si>
     <t>Energy</t>
-  </si>
-  <si>
-    <t>Ø20-601b-2_radiator_heat</t>
   </si>
   <si>
     <t>Motion</t>
@@ -397,9 +380,6 @@
   </si>
   <si>
     <t>hasProperty</t>
-  </si>
-  <si>
-    <t>Ø20-601b-2_temperature;Ø20-601b-2_CO2</t>
   </si>
   <si>
     <t>isExternal</t>
@@ -454,6 +434,75 @@
   </si>
   <si>
     <t>Co2</t>
+  </si>
+  <si>
+    <t>Air to air heat recovery;Supply fan</t>
+  </si>
+  <si>
+    <t>VE02 Primary Airflow Temperature BHR sensor</t>
+  </si>
+  <si>
+    <t>VE02 Primary Airflow Temperature AHR sensor</t>
+  </si>
+  <si>
+    <t>VE02 Primary Airflow Temperature AHC sensor</t>
+  </si>
+  <si>
+    <t>VE02 Primary Airflow Temperature AHC property</t>
+  </si>
+  <si>
+    <t>VE02 Primary Airflow Temperature AHR property</t>
+  </si>
+  <si>
+    <t>VE02 Primary Airflow Temperature BHR property</t>
+  </si>
+  <si>
+    <t>Ø20-601b-2 radiator heat property</t>
+  </si>
+  <si>
+    <t>Ø20-601b-2 damper position property</t>
+  </si>
+  <si>
+    <t>Ø20-601b-2 radiator valve position property</t>
+  </si>
+  <si>
+    <t>Ø20-601b-2 CO2 property</t>
+  </si>
+  <si>
+    <t>Ø20-601b-2 temperature property</t>
+  </si>
+  <si>
+    <t>Ø20-601b-2 temperature property;Ø20-601b-2 CO2 property</t>
+  </si>
+  <si>
+    <t>Ø20-601b-2 shading position property</t>
+  </si>
+  <si>
+    <t>VE02 Primary Airflow Temperature AHR sensor;Heating coil</t>
+  </si>
+  <si>
+    <t>VE02 Secondary Airflow Temperature BHR sensor</t>
+  </si>
+  <si>
+    <t>VE02 Primary Airflow Temperature AHC sensor;Supply fan</t>
+  </si>
+  <si>
+    <t>VE02 Primary Airflow Temperature BHR sensor;VE02 Primary Airflow Temperature AHR sensor;VE02 Secondary Airflow Temperature BHR sensor;Exhaust fan</t>
+  </si>
+  <si>
+    <t>Outdoor environment;Air to air heat recovery</t>
+  </si>
+  <si>
+    <t>Heating coil;Supply damper</t>
+  </si>
+  <si>
+    <t>Air to air heat recovery;Exhaust damper</t>
+  </si>
+  <si>
+    <t>VE02 Primary Airflow Temperature BHR property;VE02 Primary Airflow Temperature AHR property;VE02 Secondary Airflow Temperature BHR property</t>
+  </si>
+  <si>
+    <t>VE02 Secondary Airflow Temperature BHR property</t>
   </si>
 </sst>
 </file>
@@ -632,6 +681,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>323310</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>160692</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB500964-3927-4A67-BFB8-0A97850FB440}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7886700" y="1343025"/>
+          <a:ext cx="13734510" cy="6447192"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -923,7 +1021,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -934,7 +1032,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="X35" sqref="X35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,11 +1062,6 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" sqref="A2:C1048576" xr:uid="{A750DCD6-2C0D-4A1E-B416-01652FC4C907}">
-      <formula1>count_name_occurences(A2)&lt;=1</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -979,14 +1072,14 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
@@ -1009,45 +1102,45 @@
         <v>62</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="K1" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="M1" s="14" t="s">
         <v>104</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
         <v>112</v>
       </c>
-      <c r="C2" t="s">
-        <v>119</v>
-      </c>
       <c r="D2" s="8" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1062,95 +1155,163 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D904F809-0565-4493-A542-77B590BDC86C}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
         <v>114</v>
       </c>
-      <c r="B2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="B4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="B9" t="s">
         <v>118</v>
       </c>
-      <c r="B6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" t="s">
-        <v>87</v>
-      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{A9040C0C-604B-456F-96D4-0A20D2AB5CEB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{A9040C0C-604B-456F-96D4-0A20D2AB5CEB}">
       <formula1>property_instance</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6" xr:uid="{B410286B-19C8-413D-AA2F-9742B6293571}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6" xr:uid="{B410286B-19C8-413D-AA2F-9742B6293571}">
       <formula1>space_names</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1158,7 +1319,7 @@
           <x14:formula1>
             <xm:f>BuildingSpace!$A$2:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>B7:B1048576</xm:sqref>
+          <xm:sqref>C7:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1168,20 +1329,21 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E1EFB1-EA7C-414E-94A7-98027577BDF8}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>64</v>
       </c>
@@ -1191,28 +1353,37 @@
       <c r="C1" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
     </row>
   </sheetData>
@@ -1233,15 +1404,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDB24A9-A7F1-4854-93D9-EBD1381307DD}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1251,12 +1422,12 @@
         <v>64</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>70</v>
@@ -1264,15 +1435,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>81</v>
@@ -1280,7 +1451,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>86</v>
+        <v>122</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>81</v>
@@ -1288,7 +1459,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>81</v>
@@ -1296,11 +1467,46 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>88</v>
-      </c>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1318,7 +1524,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,7 +1534,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -1348,57 +1554,57 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1448,13 +1654,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1464,7 +1670,7 @@
         <v>64</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>60</v>
@@ -1472,10 +1678,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="C2">
         <v>466.54</v>
@@ -1501,7 +1707,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,8 +1715,8 @@
     <col min="1" max="1" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
@@ -1540,10 +1746,10 @@
         <v>62</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>59</v>
@@ -1617,10 +1823,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>86</v>
+        <v>122</v>
       </c>
       <c r="F2" t="s">
         <v>65</v>
@@ -1638,10 +1847,13 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>129</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>86</v>
+        <v>122</v>
       </c>
       <c r="F3" t="s">
         <v>66</v>
@@ -6662,8 +6874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F9D35B-B713-4EC3-BA55-A4EE8F2F331C}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6671,7 +6883,7 @@
     <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -6696,10 +6908,10 @@
         <v>62</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>7</v>
@@ -6743,13 +6955,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
         <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="L2">
         <f>3*515+2*572</f>
@@ -12699,7 +12911,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B48:B1048576 B2:B46" xr:uid="{CDBF1DD2-FE2B-4960-AE5E-D5DDA44A6748}">
       <formula1>heating_system_names</formula1>
     </dataValidation>
@@ -12716,7 +12928,7 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12725,7 +12937,7 @@
     <col min="2" max="2" width="13.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
@@ -12746,10 +12958,10 @@
         <v>62</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>16</v>
@@ -12784,13 +12996,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
         <v>73</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="G2">
         <f>5*0.468</f>
@@ -22137,10 +22349,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4B0EA7-434A-4CA3-97FE-A57E5232E2E7}">
-  <dimension ref="A1:C1000"/>
+  <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22148,9 +22360,11 @@
     <col min="1" max="1" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>64</v>
       </c>
@@ -22160,8 +22374,14 @@
       <c r="C1" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>75</v>
       </c>
@@ -22171,68 +22391,74 @@
       <c r="C2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f t="shared" ref="A6:A66" si="0">IF(AND(B6&lt;&gt;"",C6&lt;&gt;""),_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("HC_",B6),"_"),C6),"")</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -28144,10 +28370,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{2406BDD5-983E-4F7B-9889-A7801E93AEBE}">
       <formula1>"heating,cooling"</formula1>
     </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D3:E1048576" xr:uid="{374565C9-1149-4287-9BC4-32CC991B8BB7}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -28156,135 +28383,153 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13A142E3-535E-45D7-B544-7DE9118FD57D}">
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="G2">
-        <f>5000/3600*1.225</f>
-        <v>1.7013888888888891</v>
+      <c r="C2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>135</v>
       </c>
       <c r="I2">
         <f>5000/3600*1.225</f>
         <v>1.7013888888888891</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <f>5000/3600*1.225</f>
+        <v>1.7013888888888891</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f t="shared" ref="A6:A66" si="0">IF(B6&lt;&gt;"",_xlfn.CONCAT("HR_",B6),"")</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -34196,10 +34441,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{164381D2-0FCF-4A4E-A4F9-78C16B3F8259}">
       <formula1>ventilation_system_names</formula1>
     </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C3:D1048576" xr:uid="{7B0207D7-F0F5-45A7-B38C-70BCADF38C7F}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -34208,10 +34454,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC2999C7-12DB-42EA-8FDC-B5FA87CE6F00}">
-  <dimension ref="A1:M1000"/>
+  <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34219,19 +34465,21 @@
     <col min="1" max="1" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>64</v>
       </c>
@@ -34241,38 +34489,44 @@
       <c r="C1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>77</v>
       </c>
@@ -34282,15 +34536,18 @@
       <c r="C2" t="s">
         <v>65</v>
       </c>
-      <c r="F2">
+      <c r="D2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2">
         <f>5000/3600*1.225</f>
         <v>1.7013888888888891</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>1500</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>78</v>
       </c>
@@ -34300,51 +34557,54 @@
       <c r="C3" t="s">
         <v>66</v>
       </c>
-      <c r="F3">
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3">
         <f>5000/3600*1.225</f>
         <v>1.7013888888888891</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>1500</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
         <f t="shared" ref="A10:A66" si="0">IF(AND(B10&lt;&gt;"",C10&lt;&gt;""),_xlfn.CONCAT(_xlfn.CONCAT(_xlfn.CONCAT("F_",C10),"_"),B10),"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -40273,7 +40533,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40281,7 +40541,7 @@
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -40309,10 +40569,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -40323,10 +40583,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add Monitor class for continous commissioning
</commit_message>
<xml_diff>
--- a/twin4build/test/data/configuration_template_1space_1v_1h_0c_test_new_layout_simple_naming.xlsx
+++ b/twin4build/test/data/configuration_template_1space_1v_1h_0c_test_new_layout_simple_naming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syddanskuni-my.sharepoint.com/personal/jabj_mmmi_sdu_dk/Documents/PhD_Project_Jakob/Twin4build/python/BuildingEnergyModel/BuildingEnergyModel/twin4build/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="538" documentId="8_{AAA6B40C-6A0C-4905-8430-5C49F148860B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA16BDFB-8A35-43B0-B96C-3A615FD10DFD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E73693FB-AD66-4C1C-BA47-DFA0CC2CBC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="3" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="136">
   <si>
     <t>Ventilation system name</t>
   </si>
@@ -427,9 +427,6 @@
     <t>Damper position sensor</t>
   </si>
   <si>
-    <t>Shading position sensor</t>
-  </si>
-  <si>
     <t>Space</t>
   </si>
   <si>
@@ -689,13 +686,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>323310</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>160692</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1137,10 +1134,10 @@
         <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1155,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D904F809-0565-4493-A542-77B590BDC86C}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,10 +1189,10 @@
         <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1203,10 +1200,10 @@
         <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1214,10 +1211,10 @@
         <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1225,21 +1222,24 @@
         <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C6" t="s">
-        <v>112</v>
+        <v>119</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1247,13 +1247,13 @@
         <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1261,21 +1261,21 @@
         <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -1285,29 +1285,15 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B10" t="s">
-        <v>136</v>
-      </c>
-      <c r="D10" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A10" s="8"/>
     </row>
   </sheetData>
   <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5" xr:uid="{B410286B-19C8-413D-AA2F-9742B6293571}">
+      <formula1>space_names</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{A9040C0C-604B-456F-96D4-0A20D2AB5CEB}">
       <formula1>property_instance</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6" xr:uid="{B410286B-19C8-413D-AA2F-9742B6293571}">
-      <formula1>space_names</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1319,7 +1305,7 @@
           <x14:formula1>
             <xm:f>BuildingSpace!$A$2:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>C7:C1048576</xm:sqref>
+          <xm:sqref>C6:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1332,7 +1318,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,10 +1351,10 @@
         <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -1407,7 +1393,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,7 +1413,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>70</v>
@@ -1435,15 +1421,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>81</v>
@@ -1451,7 +1437,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>81</v>
@@ -1459,7 +1445,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>81</v>
@@ -1467,7 +1453,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>83</v>
@@ -1475,7 +1461,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
         <v>70</v>
@@ -1483,7 +1469,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" t="s">
         <v>70</v>
@@ -1491,7 +1477,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
@@ -1499,7 +1485,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
         <v>70</v>
@@ -1604,7 +1590,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1678,10 +1664,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2">
         <v>466.54</v>
@@ -1706,7 +1692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A747EB8B-49DD-40FE-8CAD-B5A7A33DF8B7}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1823,13 +1809,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F2" t="s">
         <v>65</v>
@@ -1847,13 +1833,13 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F3" t="s">
         <v>66</v>
@@ -6955,13 +6941,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
         <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L2">
         <f>3*515+2*572</f>
@@ -12996,13 +12982,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
         <v>73</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G2">
         <f>5*0.468</f>
@@ -22392,10 +22378,10 @@
         <v>67</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -28385,8 +28371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13A142E3-535E-45D7-B544-7DE9118FD57D}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28451,10 +28437,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I2">
         <f>5000/3600*1.225</f>
@@ -34537,7 +34523,7 @@
         <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H2">
         <f>5000/3600*1.225</f>
@@ -40569,10 +40555,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -40583,10 +40569,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Do changes to allow for temporary BS2023 simulation
</commit_message>
<xml_diff>
--- a/twin4build/test/data/configuration_template_1space_1v_1h_0c_test_new_layout_simple_naming.xlsx
+++ b/twin4build/test/data/configuration_template_1space_1v_1h_0c_test_new_layout_simple_naming.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{E73693FB-AD66-4C1C-BA47-DFA0CC2CBC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="8" xr2:uid="{0A98B5A4-E8E7-4876-BAF5-D3C6F6E2C062}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="3" r:id="rId1"/>
@@ -1692,7 +1692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A747EB8B-49DD-40FE-8CAD-B5A7A33DF8B7}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -40518,8 +40518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EEF019-D7A4-42FF-B5C0-3702855A99F7}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>